<commit_message>
Fix LR2 and LR3(t1)
</commit_message>
<xml_diff>
--- a/LR3/table_1_58.xlsx
+++ b/LR3/table_1_58.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63745C7A-CB6F-4395-8A97-ADB7CAFBF917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884576BF-B74A-4B23-B6E3-6D43CEE608BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -164,9 +164,6 @@
     <t>Средняя площадь, кв.м.</t>
   </si>
   <si>
-    <t>Общая сумма графы “Итого”, руб.</t>
-  </si>
-  <si>
     <t>Максимальная сумма к оплате, руб.</t>
   </si>
   <si>
@@ -183,15 +180,17 @@
   </si>
   <si>
     <t>Штраф,руб.</t>
+  </si>
+  <si>
+    <t>Общая сумма</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₽&quot;_-;\-* #,##0.00\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="#,##0\ &quot;₽&quot;"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;₽&quot;"/>
     <numFmt numFmtId="166" formatCode="#,##0.00\ [$₽-419]"/>
   </numFmts>
@@ -272,11 +271,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -559,15 +558,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
@@ -608,13 +607,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>38</v>
@@ -626,10 +625,10 @@
         <v>40</v>
       </c>
       <c r="I2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>41</v>
@@ -652,7 +651,7 @@
         <v>70</v>
       </c>
       <c r="D3" s="1">
-        <f>$A$1*1.1</f>
+        <f>A1*1.1</f>
         <v>63.800000000000004</v>
       </c>
       <c r="E3" s="5">
@@ -669,14 +668,14 @@
         <f>IF(G3&lt;=F3,0,G3-F3)</f>
         <v>0</v>
       </c>
-      <c r="I3" s="12">
-        <v>10</v>
-      </c>
-      <c r="J3" s="12">
+      <c r="I3" s="11">
+        <v>10</v>
+      </c>
+      <c r="J3" s="11">
         <f>I3*H3</f>
         <v>0</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="11">
         <f>E3+J3</f>
         <v>4466</v>
       </c>
@@ -699,6 +698,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
+        <f>C3-0.5</f>
         <v>69.5</v>
       </c>
       <c r="D4" s="1">
@@ -719,14 +719,14 @@
         <f t="shared" ref="H4:H38" si="2">IF(G4&lt;=F4,0,G4-F4)</f>
         <v>0</v>
       </c>
-      <c r="I4" s="12">
-        <v>10</v>
-      </c>
-      <c r="J4" s="12">
+      <c r="I4" s="11">
+        <v>10</v>
+      </c>
+      <c r="J4" s="11">
         <f t="shared" ref="J4:J38" si="3">I4*H4</f>
         <v>0</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="11">
         <f t="shared" ref="K4:K38" si="4">E4+J4</f>
         <v>4434.1000000000004</v>
       </c>
@@ -749,6 +749,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="1">
+        <f t="shared" ref="C5:C38" si="7">C4-0.5</f>
         <v>69</v>
       </c>
       <c r="D5" s="1">
@@ -769,14 +770,14 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I5" s="12">
-        <v>10</v>
-      </c>
-      <c r="J5" s="12">
+      <c r="I5" s="11">
+        <v>10</v>
+      </c>
+      <c r="J5" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="11">
         <f t="shared" si="4"/>
         <v>4402.2000000000007</v>
       </c>
@@ -799,6 +800,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="1">
+        <f t="shared" si="7"/>
         <v>68.5</v>
       </c>
       <c r="D6" s="1">
@@ -819,14 +821,14 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I6" s="12">
-        <v>10</v>
-      </c>
-      <c r="J6" s="12">
+      <c r="I6" s="11">
+        <v>10</v>
+      </c>
+      <c r="J6" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K6" s="12">
+      <c r="K6" s="11">
         <f t="shared" si="4"/>
         <v>4370.3</v>
       </c>
@@ -849,6 +851,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="1">
+        <f t="shared" si="7"/>
         <v>68</v>
       </c>
       <c r="D7" s="1">
@@ -869,14 +872,14 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I7" s="12">
-        <v>10</v>
-      </c>
-      <c r="J7" s="12">
+      <c r="I7" s="11">
+        <v>10</v>
+      </c>
+      <c r="J7" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="11">
         <f t="shared" si="4"/>
         <v>4338.4000000000005</v>
       </c>
@@ -899,6 +902,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="1">
+        <f t="shared" si="7"/>
         <v>67.5</v>
       </c>
       <c r="D8" s="1">
@@ -919,14 +923,14 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I8" s="12">
-        <v>10</v>
-      </c>
-      <c r="J8" s="12">
+      <c r="I8" s="11">
+        <v>10</v>
+      </c>
+      <c r="J8" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K8" s="11">
         <f t="shared" si="4"/>
         <v>4306.5</v>
       </c>
@@ -949,6 +953,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="1">
+        <f t="shared" si="7"/>
         <v>67</v>
       </c>
       <c r="D9" s="1">
@@ -969,14 +974,14 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I9" s="12">
-        <v>10</v>
-      </c>
-      <c r="J9" s="12">
+      <c r="I9" s="11">
+        <v>10</v>
+      </c>
+      <c r="J9" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K9" s="12">
+      <c r="K9" s="11">
         <f t="shared" si="4"/>
         <v>4274.6000000000004</v>
       </c>
@@ -999,6 +1004,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="1">
+        <f t="shared" si="7"/>
         <v>66.5</v>
       </c>
       <c r="D10" s="1">
@@ -1019,14 +1025,14 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I10" s="12">
-        <v>10</v>
-      </c>
-      <c r="J10" s="12">
+      <c r="I10" s="11">
+        <v>10</v>
+      </c>
+      <c r="J10" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K10" s="12">
+      <c r="K10" s="11">
         <f t="shared" si="4"/>
         <v>4242.7000000000007</v>
       </c>
@@ -1049,6 +1055,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="1">
+        <f t="shared" si="7"/>
         <v>66</v>
       </c>
       <c r="D11" s="1">
@@ -1069,14 +1076,14 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I11" s="12">
-        <v>10</v>
-      </c>
-      <c r="J11" s="12">
+      <c r="I11" s="11">
+        <v>10</v>
+      </c>
+      <c r="J11" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K11" s="12">
+      <c r="K11" s="11">
         <f t="shared" si="4"/>
         <v>4210.8</v>
       </c>
@@ -1099,6 +1106,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="1">
+        <f t="shared" si="7"/>
         <v>65.5</v>
       </c>
       <c r="D12" s="1">
@@ -1119,14 +1127,14 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="I12" s="12">
-        <v>10</v>
-      </c>
-      <c r="J12" s="12">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="K12" s="12">
+      <c r="I12" s="11">
+        <v>10</v>
+      </c>
+      <c r="J12" s="11">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="K12" s="11">
         <f t="shared" si="4"/>
         <v>4188.9000000000005</v>
       </c>
@@ -1149,6 +1157,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="1">
+        <f t="shared" si="7"/>
         <v>65</v>
       </c>
       <c r="D13" s="1">
@@ -1169,14 +1178,14 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="I13" s="12">
-        <v>10</v>
-      </c>
-      <c r="J13" s="12">
+      <c r="I13" s="11">
+        <v>10</v>
+      </c>
+      <c r="J13" s="11">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="K13" s="12">
+      <c r="K13" s="11">
         <f t="shared" si="4"/>
         <v>4167</v>
       </c>
@@ -1199,6 +1208,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="1">
+        <f t="shared" si="7"/>
         <v>64.5</v>
       </c>
       <c r="D14" s="1">
@@ -1219,14 +1229,14 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="I14" s="12">
-        <v>10</v>
-      </c>
-      <c r="J14" s="12">
+      <c r="I14" s="11">
+        <v>10</v>
+      </c>
+      <c r="J14" s="11">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="K14" s="12">
+      <c r="K14" s="11">
         <f t="shared" si="4"/>
         <v>4145.1000000000004</v>
       </c>
@@ -1249,6 +1259,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="1">
+        <f t="shared" si="7"/>
         <v>64</v>
       </c>
       <c r="D15" s="1">
@@ -1269,14 +1280,14 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="I15" s="12">
-        <v>10</v>
-      </c>
-      <c r="J15" s="12">
+      <c r="I15" s="11">
+        <v>10</v>
+      </c>
+      <c r="J15" s="11">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="K15" s="12">
+      <c r="K15" s="11">
         <f t="shared" si="4"/>
         <v>4123.2000000000007</v>
       </c>
@@ -1299,6 +1310,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="1">
+        <f t="shared" si="7"/>
         <v>63.5</v>
       </c>
       <c r="D16" s="1">
@@ -1319,14 +1331,14 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="I16" s="12">
-        <v>10</v>
-      </c>
-      <c r="J16" s="12">
+      <c r="I16" s="11">
+        <v>10</v>
+      </c>
+      <c r="J16" s="11">
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="K16" s="12">
+      <c r="K16" s="11">
         <f t="shared" si="4"/>
         <v>4101.3</v>
       </c>
@@ -1349,6 +1361,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="1">
+        <f t="shared" si="7"/>
         <v>63</v>
       </c>
       <c r="D17" s="1">
@@ -1369,14 +1382,14 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="I17" s="12">
-        <v>10</v>
-      </c>
-      <c r="J17" s="12">
+      <c r="I17" s="11">
+        <v>10</v>
+      </c>
+      <c r="J17" s="11">
         <f t="shared" si="3"/>
         <v>60</v>
       </c>
-      <c r="K17" s="12">
+      <c r="K17" s="11">
         <f t="shared" si="4"/>
         <v>4079.4</v>
       </c>
@@ -1399,6 +1412,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="1">
+        <f t="shared" si="7"/>
         <v>62.5</v>
       </c>
       <c r="D18" s="1">
@@ -1419,14 +1433,14 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="I18" s="12">
-        <v>10</v>
-      </c>
-      <c r="J18" s="12">
+      <c r="I18" s="11">
+        <v>10</v>
+      </c>
+      <c r="J18" s="11">
         <f t="shared" si="3"/>
         <v>70</v>
       </c>
-      <c r="K18" s="12">
+      <c r="K18" s="11">
         <f t="shared" si="4"/>
         <v>4057.5000000000005</v>
       </c>
@@ -1449,6 +1463,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="1">
+        <f t="shared" si="7"/>
         <v>62</v>
       </c>
       <c r="D19" s="1">
@@ -1469,14 +1484,14 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="I19" s="12">
-        <v>10</v>
-      </c>
-      <c r="J19" s="12">
+      <c r="I19" s="11">
+        <v>10</v>
+      </c>
+      <c r="J19" s="11">
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
-      <c r="K19" s="12">
+      <c r="K19" s="11">
         <f t="shared" si="4"/>
         <v>4035.6000000000004</v>
       </c>
@@ -1499,6 +1514,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="1">
+        <f t="shared" si="7"/>
         <v>61.5</v>
       </c>
       <c r="D20" s="1">
@@ -1519,14 +1535,14 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="I20" s="12">
-        <v>10</v>
-      </c>
-      <c r="J20" s="12">
+      <c r="I20" s="11">
+        <v>10</v>
+      </c>
+      <c r="J20" s="11">
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="K20" s="12">
+      <c r="K20" s="11">
         <f t="shared" si="4"/>
         <v>4013.7000000000003</v>
       </c>
@@ -1549,6 +1565,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="1">
+        <f t="shared" si="7"/>
         <v>61</v>
       </c>
       <c r="D21" s="1">
@@ -1569,14 +1586,14 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="I21" s="12">
-        <v>10</v>
-      </c>
-      <c r="J21" s="12">
+      <c r="I21" s="11">
+        <v>10</v>
+      </c>
+      <c r="J21" s="11">
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="K21" s="12">
+      <c r="K21" s="11">
         <f t="shared" si="4"/>
         <v>3991.8</v>
       </c>
@@ -1599,6 +1616,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="1">
+        <f t="shared" si="7"/>
         <v>60.5</v>
       </c>
       <c r="D22" s="1">
@@ -1619,14 +1637,14 @@
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="I22" s="12">
-        <v>10</v>
-      </c>
-      <c r="J22" s="12">
+      <c r="I22" s="11">
+        <v>10</v>
+      </c>
+      <c r="J22" s="11">
         <f t="shared" si="3"/>
         <v>110</v>
       </c>
-      <c r="K22" s="12">
+      <c r="K22" s="11">
         <f t="shared" si="4"/>
         <v>3969.9</v>
       </c>
@@ -1649,6 +1667,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="1">
+        <f t="shared" si="7"/>
         <v>60</v>
       </c>
       <c r="D23" s="1">
@@ -1669,14 +1688,14 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="I23" s="12">
-        <v>10</v>
-      </c>
-      <c r="J23" s="12">
+      <c r="I23" s="11">
+        <v>10</v>
+      </c>
+      <c r="J23" s="11">
         <f t="shared" si="3"/>
         <v>120</v>
       </c>
-      <c r="K23" s="12">
+      <c r="K23" s="11">
         <f t="shared" si="4"/>
         <v>3948.0000000000005</v>
       </c>
@@ -1699,6 +1718,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="1">
+        <f t="shared" si="7"/>
         <v>59.5</v>
       </c>
       <c r="D24" s="1">
@@ -1719,14 +1739,14 @@
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="I24" s="12">
-        <v>10</v>
-      </c>
-      <c r="J24" s="12">
+      <c r="I24" s="11">
+        <v>10</v>
+      </c>
+      <c r="J24" s="11">
         <f t="shared" si="3"/>
         <v>130</v>
       </c>
-      <c r="K24" s="12">
+      <c r="K24" s="11">
         <f t="shared" si="4"/>
         <v>3926.1000000000004</v>
       </c>
@@ -1749,6 +1769,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="1">
+        <f t="shared" si="7"/>
         <v>59</v>
       </c>
       <c r="D25" s="1">
@@ -1769,14 +1790,14 @@
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="I25" s="12">
-        <v>10</v>
-      </c>
-      <c r="J25" s="12">
+      <c r="I25" s="11">
+        <v>10</v>
+      </c>
+      <c r="J25" s="11">
         <f t="shared" si="3"/>
         <v>140</v>
       </c>
-      <c r="K25" s="12">
+      <c r="K25" s="11">
         <f t="shared" si="4"/>
         <v>3904.2000000000003</v>
       </c>
@@ -1799,6 +1820,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="1">
+        <f t="shared" si="7"/>
         <v>58.5</v>
       </c>
       <c r="D26" s="1">
@@ -1819,14 +1841,14 @@
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="I26" s="12">
-        <v>10</v>
-      </c>
-      <c r="J26" s="12">
+      <c r="I26" s="11">
+        <v>10</v>
+      </c>
+      <c r="J26" s="11">
         <f t="shared" si="3"/>
         <v>150</v>
       </c>
-      <c r="K26" s="12">
+      <c r="K26" s="11">
         <f t="shared" si="4"/>
         <v>3882.3</v>
       </c>
@@ -1849,6 +1871,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="1">
+        <f t="shared" si="7"/>
         <v>58</v>
       </c>
       <c r="D27" s="1">
@@ -1869,14 +1892,14 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="I27" s="12">
-        <v>10</v>
-      </c>
-      <c r="J27" s="12">
+      <c r="I27" s="11">
+        <v>10</v>
+      </c>
+      <c r="J27" s="11">
         <f t="shared" si="3"/>
         <v>160</v>
       </c>
-      <c r="K27" s="12">
+      <c r="K27" s="11">
         <f t="shared" si="4"/>
         <v>3860.4</v>
       </c>
@@ -1899,6 +1922,7 @@
         <v>27</v>
       </c>
       <c r="C28" s="1">
+        <f t="shared" si="7"/>
         <v>57.5</v>
       </c>
       <c r="D28" s="1">
@@ -1919,14 +1943,14 @@
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="I28" s="12">
-        <v>10</v>
-      </c>
-      <c r="J28" s="12">
+      <c r="I28" s="11">
+        <v>10</v>
+      </c>
+      <c r="J28" s="11">
         <f t="shared" si="3"/>
         <v>170</v>
       </c>
-      <c r="K28" s="12">
+      <c r="K28" s="11">
         <f t="shared" si="4"/>
         <v>3838.5000000000005</v>
       </c>
@@ -1949,6 +1973,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="1">
+        <f t="shared" si="7"/>
         <v>57</v>
       </c>
       <c r="D29" s="1">
@@ -1969,14 +1994,14 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="I29" s="12">
-        <v>10</v>
-      </c>
-      <c r="J29" s="12">
+      <c r="I29" s="11">
+        <v>10</v>
+      </c>
+      <c r="J29" s="11">
         <f t="shared" si="3"/>
         <v>180</v>
       </c>
-      <c r="K29" s="12">
+      <c r="K29" s="11">
         <f t="shared" si="4"/>
         <v>3816.6000000000004</v>
       </c>
@@ -1999,6 +2024,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="1">
+        <f t="shared" si="7"/>
         <v>56.5</v>
       </c>
       <c r="D30" s="1">
@@ -2019,14 +2045,14 @@
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="I30" s="12">
-        <v>10</v>
-      </c>
-      <c r="J30" s="12">
+      <c r="I30" s="11">
+        <v>10</v>
+      </c>
+      <c r="J30" s="11">
         <f t="shared" si="3"/>
         <v>190</v>
       </c>
-      <c r="K30" s="12">
+      <c r="K30" s="11">
         <f t="shared" si="4"/>
         <v>3794.7000000000003</v>
       </c>
@@ -2049,6 +2075,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="1">
+        <f t="shared" si="7"/>
         <v>56</v>
       </c>
       <c r="D31" s="1">
@@ -2069,14 +2096,14 @@
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="I31" s="12">
-        <v>10</v>
-      </c>
-      <c r="J31" s="12">
+      <c r="I31" s="11">
+        <v>10</v>
+      </c>
+      <c r="J31" s="11">
         <f t="shared" si="3"/>
         <v>200</v>
       </c>
-      <c r="K31" s="12">
+      <c r="K31" s="11">
         <f t="shared" si="4"/>
         <v>3772.8</v>
       </c>
@@ -2099,6 +2126,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="1">
+        <f t="shared" si="7"/>
         <v>55.5</v>
       </c>
       <c r="D32" s="1">
@@ -2119,14 +2147,14 @@
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="I32" s="12">
-        <v>10</v>
-      </c>
-      <c r="J32" s="12">
+      <c r="I32" s="11">
+        <v>10</v>
+      </c>
+      <c r="J32" s="11">
         <f t="shared" si="3"/>
         <v>210</v>
       </c>
-      <c r="K32" s="12">
+      <c r="K32" s="11">
         <f t="shared" si="4"/>
         <v>3750.9</v>
       </c>
@@ -2149,6 +2177,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="1">
+        <f t="shared" si="7"/>
         <v>55</v>
       </c>
       <c r="D33" s="1">
@@ -2169,14 +2198,14 @@
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="I33" s="12">
-        <v>10</v>
-      </c>
-      <c r="J33" s="12">
+      <c r="I33" s="11">
+        <v>10</v>
+      </c>
+      <c r="J33" s="11">
         <f t="shared" si="3"/>
         <v>220</v>
       </c>
-      <c r="K33" s="12">
+      <c r="K33" s="11">
         <f t="shared" si="4"/>
         <v>3729.0000000000005</v>
       </c>
@@ -2199,6 +2228,7 @@
         <v>33</v>
       </c>
       <c r="C34" s="1">
+        <f t="shared" si="7"/>
         <v>54.5</v>
       </c>
       <c r="D34" s="1">
@@ -2219,14 +2249,14 @@
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="I34" s="12">
-        <v>10</v>
-      </c>
-      <c r="J34" s="12">
+      <c r="I34" s="11">
+        <v>10</v>
+      </c>
+      <c r="J34" s="11">
         <f t="shared" si="3"/>
         <v>230</v>
       </c>
-      <c r="K34" s="12">
+      <c r="K34" s="11">
         <f t="shared" si="4"/>
         <v>3707.1000000000004</v>
       </c>
@@ -2249,10 +2279,11 @@
         <v>34</v>
       </c>
       <c r="C35" s="1">
+        <f t="shared" si="7"/>
         <v>54</v>
       </c>
       <c r="D35" s="1">
-        <f>$D$3/2</f>
+        <f>D3/2</f>
         <v>31.900000000000002</v>
       </c>
       <c r="E35" s="5">
@@ -2269,14 +2300,14 @@
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="I35" s="12">
-        <v>10</v>
-      </c>
-      <c r="J35" s="12">
+      <c r="I35" s="11">
+        <v>10</v>
+      </c>
+      <c r="J35" s="11">
         <f t="shared" si="3"/>
         <v>240</v>
       </c>
-      <c r="K35" s="12">
+      <c r="K35" s="11">
         <f t="shared" si="4"/>
         <v>1962.6000000000001</v>
       </c>
@@ -2299,10 +2330,11 @@
         <v>35</v>
       </c>
       <c r="C36" s="1">
+        <f t="shared" si="7"/>
         <v>53.5</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" ref="D36:D38" si="7">$D$3/2</f>
+        <f>D3/2</f>
         <v>31.900000000000002</v>
       </c>
       <c r="E36" s="5">
@@ -2319,14 +2351,14 @@
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="I36" s="12">
-        <v>10</v>
-      </c>
-      <c r="J36" s="12">
+      <c r="I36" s="11">
+        <v>10</v>
+      </c>
+      <c r="J36" s="11">
         <f t="shared" si="3"/>
         <v>250</v>
       </c>
-      <c r="K36" s="12">
+      <c r="K36" s="11">
         <f t="shared" si="4"/>
         <v>1956.65</v>
       </c>
@@ -2349,10 +2381,11 @@
         <v>36</v>
       </c>
       <c r="C37" s="1">
+        <f t="shared" si="7"/>
         <v>53</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" si="7"/>
+        <f>D3/2</f>
         <v>31.900000000000002</v>
       </c>
       <c r="E37" s="5">
@@ -2369,14 +2402,14 @@
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="I37" s="12">
-        <v>10</v>
-      </c>
-      <c r="J37" s="12">
+      <c r="I37" s="11">
+        <v>10</v>
+      </c>
+      <c r="J37" s="11">
         <f t="shared" si="3"/>
         <v>260</v>
       </c>
-      <c r="K37" s="12">
+      <c r="K37" s="11">
         <f t="shared" si="4"/>
         <v>1950.7</v>
       </c>
@@ -2399,10 +2432,11 @@
         <v>37</v>
       </c>
       <c r="C38" s="1">
+        <f t="shared" si="7"/>
         <v>52.5</v>
       </c>
       <c r="D38" s="1">
-        <f t="shared" si="7"/>
+        <f>D3/2</f>
         <v>31.900000000000002</v>
       </c>
       <c r="E38" s="5">
@@ -2419,14 +2453,14 @@
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="I38" s="12">
-        <v>10</v>
-      </c>
-      <c r="J38" s="12">
+      <c r="I38" s="11">
+        <v>10</v>
+      </c>
+      <c r="J38" s="11">
         <f t="shared" si="3"/>
         <v>270</v>
       </c>
-      <c r="K38" s="12">
+      <c r="K38" s="11">
         <f t="shared" si="4"/>
         <v>1944.75</v>
       </c>
@@ -2459,14 +2493,14 @@
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
     </row>
-    <row r="40" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C40" s="10">
-        <f>SUM(K3:K38)</f>
-        <v>137664.30000000002</v>
+        <v>50</v>
+      </c>
+      <c r="C40" s="12">
+        <f>FLOOR(SUM(K3:K38),1)</f>
+        <v>137664</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -2485,7 +2519,7 @@
     </row>
     <row r="41" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="10" t="s">
         <v>43</v>
       </c>
       <c r="C41" s="1">
@@ -2509,7 +2543,7 @@
     </row>
     <row r="42" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="10" t="s">
         <v>42</v>
       </c>
       <c r="C42" s="1">
@@ -2533,8 +2567,8 @@
     </row>
     <row r="43" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
-      <c r="B43" s="11" t="s">
-        <v>45</v>
+      <c r="B43" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="C43" s="7">
         <f>MAX(K3:K38)</f>

</xml_diff>